<commit_message>
Quartile Lines and transform function
added vertical lines with text to show the inner quartiles (Q1,Q2,Q3) of
the bandwidth, latency, and framerate cuts.
Added a transform function to abstract the transformation process for
bandwidth and latency into a function
</commit_message>
<xml_diff>
--- a/mahalTest.xlsx
+++ b/mahalTest.xlsx
@@ -55,13 +55,31 @@
     <t>iscomplete</t>
   </si>
   <si>
+    <t>0b826a3f-cca2-4048-b9a4-45c37dfe1698</t>
+  </si>
+  <si>
+    <t>0ce22d81-edba-4cee-9e83-6b771de9e8ed</t>
+  </si>
+  <si>
+    <t>ee1c2ec1-eb20-4696-a339-cc36b58e124d</t>
+  </si>
+  <si>
     <t>4f723324-27d7-4a9f-96f6-97bc425eb237</t>
   </si>
   <si>
-    <t>0b826a3f-cca2-4048-b9a4-45c37dfe1698</t>
-  </si>
-  <si>
-    <t>0ce22d81-edba-4cee-9e83-6b771de9e8ed</t>
+    <t>50833a5a-eca4-49fe-b011-53afd43d4814</t>
+  </si>
+  <si>
+    <t>8c936581-975d-42d0-aca2-2d25117aca21</t>
+  </si>
+  <si>
+    <t>0b1a7d84-613f-476b-b322-6bec7821f60c</t>
+  </si>
+  <si>
+    <t>a658be8e-1ccb-4296-812f-a997819f7b00</t>
+  </si>
+  <si>
+    <t>5449e5af-ec76-4183-aaac-944e32a9bee0</t>
   </si>
   <si>
     <t>19f430f3-34d1-4d1b-b320-ac725def0a9c</t>
@@ -79,33 +97,30 @@
     <t>36ec2032-3a1d-4fbb-88fd-2b50a14461e6</t>
   </si>
   <si>
-    <t>ee1c2ec1-eb20-4696-a339-cc36b58e124d</t>
-  </si>
-  <si>
     <t>f1306d5c-7d10-4ccf-87dd-960272fd3e5e</t>
   </si>
   <si>
-    <t>50833a5a-eca4-49fe-b011-53afd43d4814</t>
-  </si>
-  <si>
     <t>0cacb2c9-3121-4d8e-b95d-15d1919e4e2f</t>
   </si>
   <si>
-    <t>8c936581-975d-42d0-aca2-2d25117aca21</t>
-  </si>
-  <si>
-    <t>0b1a7d84-613f-476b-b322-6bec7821f60c</t>
-  </si>
-  <si>
-    <t>a658be8e-1ccb-4296-812f-a997819f7b00</t>
-  </si>
-  <si>
-    <t>5449e5af-ec76-4183-aaac-944e32a9bee0</t>
-  </si>
-  <si>
     <t>2a0690f9-1ec7-4cf2-af26-0d12e250bcaa</t>
   </si>
   <si>
+    <t>dac9fda5-b765-4395-b834-188960d6d464</t>
+  </si>
+  <si>
+    <t>10386ba5-3cde-4ace-badf-016813528769</t>
+  </si>
+  <si>
+    <t>5d0cf60f-4e17-48b9-93c8-2b7a778cb2c3</t>
+  </si>
+  <si>
+    <t>18e963ae-7dac-478f-9098-f7da859762f6</t>
+  </si>
+  <si>
+    <t>0c533ea6-5a78-49ee-a577-81ae51bd8238</t>
+  </si>
+  <si>
     <t>14625c3d-1eb3-426a-ba1a-c5a6e79f0f64</t>
   </si>
   <si>
@@ -136,28 +151,31 @@
     <t>5460b966-8668-46ab-aede-910a8bc16c4a</t>
   </si>
   <si>
-    <t>dac9fda5-b765-4395-b834-188960d6d464</t>
-  </si>
-  <si>
-    <t>10386ba5-3cde-4ace-badf-016813528769</t>
-  </si>
-  <si>
-    <t>5d0cf60f-4e17-48b9-93c8-2b7a778cb2c3</t>
-  </si>
-  <si>
-    <t>18e963ae-7dac-478f-9098-f7da859762f6</t>
-  </si>
-  <si>
-    <t>0c533ea6-5a78-49ee-a577-81ae51bd8238</t>
+    <t>c9850c39-cc7c-4e7f-88b5-cb7f06e1ec88</t>
+  </si>
+  <si>
+    <t>b9b4f37b-82dc-48a3-8f82-7f169d26ff23</t>
+  </si>
+  <si>
+    <t>8199256c-d8c4-493c-a89e-e2414592c044</t>
   </si>
   <si>
     <t>33cd9aab-f97b-4902-8fb2-0595e96109f6</t>
   </si>
   <si>
-    <t>c9850c39-cc7c-4e7f-88b5-cb7f06e1ec88</t>
-  </si>
-  <si>
-    <t>b9b4f37b-82dc-48a3-8f82-7f169d26ff23</t>
+    <t>b6f40af4-013c-4f16-87a0-b3540d113d90</t>
+  </si>
+  <si>
+    <t>0d2d1a26-2681-44df-8311-471cb2299f90</t>
+  </si>
+  <si>
+    <t>addb57fc-b820-4caf-b8f0-c0f81d16c466</t>
+  </si>
+  <si>
+    <t>5dc3d313-2645-49b2-968e-679a0ab7d50c</t>
+  </si>
+  <si>
+    <t>2996360a-688d-4dfc-aec5-76e46e207833</t>
   </si>
   <si>
     <t>066fb243-eb2a-4d43-8138-a3cf92af1e5e</t>
@@ -175,33 +193,30 @@
     <t>c25b713a-a5d0-4a98-a5ea-727bd53bc956</t>
   </si>
   <si>
-    <t>8199256c-d8c4-493c-a89e-e2414592c044</t>
-  </si>
-  <si>
     <t>0920313e-1708-4a90-9058-44d60a72ce34</t>
   </si>
   <si>
-    <t>b6f40af4-013c-4f16-87a0-b3540d113d90</t>
-  </si>
-  <si>
     <t>c29b26cb-869c-4d5b-8e73-cfb94c009cea</t>
   </si>
   <si>
-    <t>0d2d1a26-2681-44df-8311-471cb2299f90</t>
-  </si>
-  <si>
-    <t>addb57fc-b820-4caf-b8f0-c0f81d16c466</t>
-  </si>
-  <si>
-    <t>5dc3d313-2645-49b2-968e-679a0ab7d50c</t>
-  </si>
-  <si>
-    <t>2996360a-688d-4dfc-aec5-76e46e207833</t>
-  </si>
-  <si>
     <t>2f337c9e-601e-4650-91ce-86cac3e1e9cb</t>
   </si>
   <si>
+    <t>3e69e2c3-09ae-4b94-adda-a371344e6bab</t>
+  </si>
+  <si>
+    <t>ba283d16-ec85-4648-b43c-5372d4115057</t>
+  </si>
+  <si>
+    <t>68c636bb-33c6-4aac-acdf-affee9145638</t>
+  </si>
+  <si>
+    <t>adc6af90-a256-496f-b9d9-255e93e21140</t>
+  </si>
+  <si>
+    <t>9cb4e416-ef70-4225-9e4b-2e1b90553e79</t>
+  </si>
+  <si>
     <t>3cb7bc1c-c723-401b-bf72-b569fdb17317</t>
   </si>
   <si>
@@ -232,21 +247,6 @@
     <t>db2b02fa-7025-4585-b429-aa32609fe176</t>
   </si>
   <si>
-    <t>3e69e2c3-09ae-4b94-adda-a371344e6bab</t>
-  </si>
-  <si>
-    <t>ba283d16-ec85-4648-b43c-5372d4115057</t>
-  </si>
-  <si>
-    <t>68c636bb-33c6-4aac-acdf-affee9145638</t>
-  </si>
-  <si>
-    <t>adc6af90-a256-496f-b9d9-255e93e21140</t>
-  </si>
-  <si>
-    <t>9cb4e416-ef70-4225-9e4b-2e1b90553e79</t>
-  </si>
-  <si>
     <t>b8c7f3f0-38d2-4528-9fee-23fba37a4569</t>
   </si>
   <si>
@@ -256,13 +256,31 @@
     <t>978baf61-658d-4665-aa48-168f044698a0</t>
   </si>
   <si>
+    <t>6RxlqelrREND3yYw</t>
+  </si>
+  <si>
+    <t>BQn1KP1vL0QDk3rj</t>
+  </si>
+  <si>
+    <t>XmaYgDGWAobDBdVJ</t>
+  </si>
+  <si>
     <t>1kl5Xz8vkYgPEB8m</t>
   </si>
   <si>
-    <t>6RxlqelrREND3yYw</t>
-  </si>
-  <si>
-    <t>BQn1KP1vL0QDk3rj</t>
+    <t>XAJL7PLW6QneRZGb</t>
+  </si>
+  <si>
+    <t>Q6Abwz4vJl2PLMJ4</t>
+  </si>
+  <si>
+    <t>EKR5LDo5V19eV136</t>
+  </si>
+  <si>
+    <t>r54dOPgQOk4zLRJ9</t>
+  </si>
+  <si>
+    <t>BQn1KP1vnXNDk3rj</t>
   </si>
   <si>
     <t>opM97DAWmjJe3E6a</t>
@@ -280,33 +298,30 @@
     <t>nMOARz2vNWbzmGN0</t>
   </si>
   <si>
-    <t>XmaYgDGWAobDBdVJ</t>
-  </si>
-  <si>
     <t>9MOwmzYolOXPq5r1</t>
   </si>
   <si>
-    <t>XAJL7PLW6QneRZGb</t>
-  </si>
-  <si>
     <t>yWrpbeXWOaMzKanm</t>
   </si>
   <si>
-    <t>Q6Abwz4vJl2PLMJ4</t>
-  </si>
-  <si>
-    <t>EKR5LDo5V19eV136</t>
-  </si>
-  <si>
-    <t>r54dOPgQOk4zLRJ9</t>
-  </si>
-  <si>
-    <t>BQn1KP1vnXNDk3rj</t>
-  </si>
-  <si>
     <t>rnKxGPdbEo3zby6Y</t>
   </si>
   <si>
+    <t>nMOARz2vWjbzmGN0</t>
+  </si>
+  <si>
+    <t>LqMnJPvBVx4P3vgj</t>
+  </si>
+  <si>
+    <t>XmaYgDGWxZRDBdVJ</t>
+  </si>
+  <si>
+    <t>G1KqyD6bpp9DAw0J</t>
+  </si>
+  <si>
+    <t>Q6Abwz4vJL4PLMJ4</t>
+  </si>
+  <si>
     <t>XAJL7PLWN1veRZGb</t>
   </si>
   <si>
@@ -335,21 +350,6 @@
   </si>
   <si>
     <t>BQn1KP1vny1Dk3rj</t>
-  </si>
-  <si>
-    <t>nMOARz2vWjbzmGN0</t>
-  </si>
-  <si>
-    <t>LqMnJPvBVx4P3vgj</t>
-  </si>
-  <si>
-    <t>XmaYgDGWxZRDBdVJ</t>
-  </si>
-  <si>
-    <t>G1KqyD6bpp9DAw0J</t>
-  </si>
-  <si>
-    <t>Q6Abwz4vJL4PLMJ4</t>
   </si>
   <si>
     <t>4bc154fd-6429-444e-b589-4b3b7cf1bda6</t>
@@ -759,7 +759,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>4347</v>
+        <v>4375</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -783,19 +783,19 @@
         <v>112</v>
       </c>
       <c r="I2">
-        <v>264</v>
+        <v>1218</v>
       </c>
       <c r="J2">
-        <v>326</v>
+        <v>696</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L2">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M2">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1">
-        <v>4613</v>
+        <v>4387</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -827,19 +827,19 @@
         <v>112</v>
       </c>
       <c r="I3">
-        <v>1218</v>
+        <v>885</v>
       </c>
       <c r="J3">
-        <v>696</v>
+        <v>534</v>
       </c>
       <c r="K3">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="L3">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="M3">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="N3" t="b">
         <v>1</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1">
-        <v>4652</v>
+        <v>4548</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -871,19 +871,19 @@
         <v>112</v>
       </c>
       <c r="I4">
-        <v>885</v>
+        <v>205</v>
       </c>
       <c r="J4">
-        <v>534</v>
+        <v>323</v>
       </c>
       <c r="K4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L4">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M4">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1">
-        <v>4691</v>
+        <v>4624</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -915,19 +915,19 @@
         <v>112</v>
       </c>
       <c r="I5">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="J5">
-        <v>548</v>
+        <v>326</v>
       </c>
       <c r="K5">
         <v>8</v>
       </c>
       <c r="L5">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M5">
-        <v>94</v>
+        <v>182</v>
       </c>
       <c r="N5" t="b">
         <v>1</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1">
-        <v>4697</v>
+        <v>4646</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -959,19 +959,19 @@
         <v>112</v>
       </c>
       <c r="I6">
-        <v>456</v>
+        <v>103</v>
       </c>
       <c r="J6">
-        <v>877</v>
+        <v>186</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="M6">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>4725</v>
+        <v>4716</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1003,19 +1003,19 @@
         <v>112</v>
       </c>
       <c r="I7">
-        <v>84</v>
+        <v>600</v>
       </c>
       <c r="J7">
-        <v>484</v>
+        <v>39</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M7">
-        <v>34</v>
+        <v>370</v>
       </c>
       <c r="N7" t="b">
         <v>1</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1">
-        <v>4732</v>
+        <v>4815</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1047,19 +1047,19 @@
         <v>112</v>
       </c>
       <c r="I8">
-        <v>132</v>
+        <v>247</v>
       </c>
       <c r="J8">
-        <v>277</v>
+        <v>206</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L8">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M8">
-        <v>544</v>
+        <v>66</v>
       </c>
       <c r="N8" t="b">
         <v>1</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1">
-        <v>4735</v>
+        <v>4820</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1091,19 +1091,19 @@
         <v>112</v>
       </c>
       <c r="I9">
-        <v>493</v>
+        <v>277</v>
       </c>
       <c r="J9">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="K9">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="L9">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="M9">
-        <v>62</v>
+        <v>310</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1">
-        <v>4813</v>
+        <v>4971</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
@@ -1135,19 +1135,19 @@
         <v>112</v>
       </c>
       <c r="I10">
-        <v>205</v>
+        <v>634</v>
       </c>
       <c r="J10">
-        <v>323</v>
+        <v>738</v>
       </c>
       <c r="K10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L10">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="M10">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="N10" t="b">
         <v>1</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1">
-        <v>4838</v>
+        <v>4995</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -1179,19 +1179,19 @@
         <v>112</v>
       </c>
       <c r="I11">
-        <v>155</v>
+        <v>256</v>
       </c>
       <c r="J11">
-        <v>392</v>
+        <v>548</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L11">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="M11">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="N11" t="b">
         <v>1</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1">
-        <v>4884</v>
+        <v>5001</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1223,19 +1223,19 @@
         <v>112</v>
       </c>
       <c r="I12">
-        <v>103</v>
+        <v>456</v>
       </c>
       <c r="J12">
-        <v>186</v>
+        <v>877</v>
       </c>
       <c r="K12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L12">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M12">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1">
-        <v>4956</v>
+        <v>5002</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -1267,19 +1267,19 @@
         <v>112</v>
       </c>
       <c r="I13">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="J13">
-        <v>365</v>
+        <v>484</v>
       </c>
       <c r="K13">
         <v>4</v>
       </c>
       <c r="L13">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="M13">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="N13" t="b">
         <v>1</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1">
-        <v>4981</v>
+        <v>5009</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -1311,19 +1311,19 @@
         <v>112</v>
       </c>
       <c r="I14">
-        <v>600</v>
+        <v>132</v>
       </c>
       <c r="J14">
-        <v>39</v>
+        <v>277</v>
       </c>
       <c r="K14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M14">
-        <v>370</v>
+        <v>544</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1">
-        <v>5080</v>
+        <v>5012</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -1355,19 +1355,19 @@
         <v>112</v>
       </c>
       <c r="I15">
-        <v>247</v>
+        <v>493</v>
       </c>
       <c r="J15">
-        <v>206</v>
+        <v>44</v>
       </c>
       <c r="K15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L15">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="M15">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N15" t="b">
         <v>1</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1">
-        <v>5085</v>
+        <v>5115</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
@@ -1399,19 +1399,19 @@
         <v>112</v>
       </c>
       <c r="I16">
-        <v>277</v>
+        <v>155</v>
       </c>
       <c r="J16">
-        <v>30</v>
+        <v>392</v>
       </c>
       <c r="K16">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="L16">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="M16">
-        <v>310</v>
+        <v>120</v>
       </c>
       <c r="N16" t="b">
         <v>1</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1">
-        <v>5209</v>
+        <v>5233</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -1443,19 +1443,19 @@
         <v>112</v>
       </c>
       <c r="I17">
-        <v>634</v>
+        <v>143</v>
       </c>
       <c r="J17">
-        <v>738</v>
+        <v>365</v>
       </c>
       <c r="K17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L17">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M17">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="N17" t="b">
         <v>1</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1">
-        <v>11209</v>
+        <v>11177</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1">
-        <v>11276</v>
+        <v>11617</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -1531,19 +1531,19 @@
         <v>112</v>
       </c>
       <c r="I19">
-        <v>338</v>
+        <v>2218</v>
       </c>
       <c r="J19">
-        <v>26</v>
+        <v>729</v>
       </c>
       <c r="K19">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L19">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M19">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="N19" t="b">
         <v>1</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1">
-        <v>11315</v>
+        <v>11659</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -1575,19 +1575,19 @@
         <v>112</v>
       </c>
       <c r="I20">
-        <v>245</v>
+        <v>108</v>
       </c>
       <c r="J20">
-        <v>270</v>
+        <v>413</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M20">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="1">
-        <v>11339</v>
+        <v>11662</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
@@ -1619,19 +1619,19 @@
         <v>112</v>
       </c>
       <c r="I21">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="J21">
-        <v>340</v>
+        <v>161</v>
       </c>
       <c r="K21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L21">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="M21">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="N21" t="b">
         <v>1</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1">
-        <v>11358</v>
+        <v>11729</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
@@ -1663,19 +1663,19 @@
         <v>112</v>
       </c>
       <c r="I22">
-        <v>2270</v>
+        <v>693</v>
       </c>
       <c r="J22">
-        <v>324</v>
+        <v>433</v>
       </c>
       <c r="K22">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="L22">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M22">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="N22" t="b">
         <v>1</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1">
-        <v>11390</v>
+        <v>11730</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -1707,19 +1707,19 @@
         <v>112</v>
       </c>
       <c r="I23">
-        <v>241</v>
+        <v>2014</v>
       </c>
       <c r="J23">
-        <v>154</v>
+        <v>275</v>
       </c>
       <c r="K23">
         <v>8</v>
       </c>
       <c r="L23">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M23">
-        <v>206</v>
+        <v>100</v>
       </c>
       <c r="N23" t="b">
         <v>1</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1">
-        <v>11429</v>
+        <v>12729</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
@@ -1751,19 +1751,19 @@
         <v>112</v>
       </c>
       <c r="I24">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J24">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="K24">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L24">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="M24">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="N24" t="b">
         <v>1</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="1">
-        <v>11443</v>
+        <v>12768</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
@@ -1795,19 +1795,19 @@
         <v>112</v>
       </c>
       <c r="I25">
-        <v>2014</v>
+        <v>245</v>
       </c>
       <c r="J25">
-        <v>316</v>
+        <v>270</v>
       </c>
       <c r="K25">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="L25">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="M25">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="1">
-        <v>11511</v>
+        <v>12792</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>
@@ -1839,19 +1839,19 @@
         <v>112</v>
       </c>
       <c r="I26">
-        <v>335</v>
+        <v>208</v>
       </c>
       <c r="J26">
-        <v>1962</v>
+        <v>340</v>
       </c>
       <c r="K26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L26">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="M26">
-        <v>178</v>
+        <v>278</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1">
-        <v>11576</v>
+        <v>12811</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
@@ -1883,19 +1883,19 @@
         <v>112</v>
       </c>
       <c r="I27">
-        <v>688</v>
+        <v>2270</v>
       </c>
       <c r="J27">
-        <v>2046</v>
+        <v>324</v>
       </c>
       <c r="K27">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="L27">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="M27">
-        <v>254</v>
+        <v>64</v>
       </c>
       <c r="N27" t="b">
         <v>1</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="1">
-        <v>11614</v>
+        <v>12843</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
@@ -1927,19 +1927,19 @@
         <v>112</v>
       </c>
       <c r="I28">
-        <v>751</v>
+        <v>241</v>
       </c>
       <c r="J28">
-        <v>29</v>
+        <v>154</v>
       </c>
       <c r="K28">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="L28">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M28">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="N28" t="b">
         <v>1</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1">
-        <v>12708</v>
+        <v>12882</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -1971,19 +1971,19 @@
         <v>112</v>
       </c>
       <c r="I29">
-        <v>2218</v>
+        <v>344</v>
       </c>
       <c r="J29">
-        <v>729</v>
+        <v>81</v>
       </c>
       <c r="K29">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L29">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M29">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="N29" t="b">
         <v>1</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="1">
-        <v>12750</v>
+        <v>12896</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
@@ -2015,19 +2015,19 @@
         <v>112</v>
       </c>
       <c r="I30">
+        <v>2014</v>
+      </c>
+      <c r="J30">
+        <v>316</v>
+      </c>
+      <c r="K30">
+        <v>14</v>
+      </c>
+      <c r="L30">
+        <v>25</v>
+      </c>
+      <c r="M30">
         <v>108</v>
-      </c>
-      <c r="J30">
-        <v>413</v>
-      </c>
-      <c r="K30">
-        <v>4</v>
-      </c>
-      <c r="L30">
-        <v>41</v>
-      </c>
-      <c r="M30">
-        <v>72</v>
       </c>
       <c r="N30" t="b">
         <v>1</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="1">
-        <v>12753</v>
+        <v>12964</v>
       </c>
       <c r="B31" t="s">
         <v>42</v>
@@ -2059,19 +2059,19 @@
         <v>112</v>
       </c>
       <c r="I31">
-        <v>260</v>
+        <v>335</v>
       </c>
       <c r="J31">
-        <v>161</v>
+        <v>1962</v>
       </c>
       <c r="K31">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L31">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="M31">
-        <v>250</v>
+        <v>178</v>
       </c>
       <c r="N31" t="b">
         <v>1</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="1">
-        <v>12820</v>
+        <v>13029</v>
       </c>
       <c r="B32" t="s">
         <v>43</v>
@@ -2103,19 +2103,19 @@
         <v>112</v>
       </c>
       <c r="I32">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="J32">
-        <v>433</v>
+        <v>2046</v>
       </c>
       <c r="K32">
         <v>4</v>
       </c>
       <c r="L32">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="M32">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="N32" t="b">
         <v>1</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="1">
-        <v>12821</v>
+        <v>13067</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
@@ -2147,19 +2147,19 @@
         <v>112</v>
       </c>
       <c r="I33">
-        <v>2014</v>
+        <v>751</v>
       </c>
       <c r="J33">
-        <v>275</v>
+        <v>29</v>
       </c>
       <c r="K33">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L33">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="M33">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="N33" t="b">
         <v>1</v>

</xml_diff>